<commit_message>
start the code of DW
</commit_message>
<xml_diff>
--- a/Demosaic/sketchMap.xlsx
+++ b/Demosaic/sketchMap.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fred\ISP\ISPAlgorithmStudy\Demosaic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISP\PersonalProjects\ISPAlgorithmStudy\Demosaic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC80AFE-3385-4DCD-8ACB-8A15E5867346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,7 +73,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -347,11 +346,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -414,6 +546,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -429,235 +575,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>202406</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>172642</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>107156</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>113110</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="直接箭头连接符 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8655D055-253B-4AF6-B3D1-DCB86ED67DF8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="23348156" y="6554392"/>
-          <a:ext cx="333375" cy="339327"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>327422</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>125017</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>196453</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>130969</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="直接箭头连接符 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FE2895F-7A99-43FE-B929-4E594567CB80}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="23901797" y="6506767"/>
-          <a:ext cx="297656" cy="404811"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>307183</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>140494</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>172640</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="直接箭头连接符 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00AE730C-5D6D-4FBF-9339-246020AB1B58}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="23336250" y="7087792"/>
-          <a:ext cx="378619" cy="264317"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>327422</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>291703</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>184548</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>196453</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="直接箭头连接符 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1DBDD91-5A0B-46F6-B931-DA4A521057A9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="23901797" y="7072312"/>
-          <a:ext cx="285751" cy="303610"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -922,7 +839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:BH38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AS14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
@@ -1159,11 +1076,11 @@
       <c r="AK16" s="23"/>
       <c r="BA16" s="2"/>
       <c r="BB16" s="3"/>
-      <c r="BC16" s="2"/>
-      <c r="BD16" s="3"/>
-      <c r="BE16" s="2"/>
-      <c r="BF16" s="3"/>
-      <c r="BG16" s="2"/>
+      <c r="BC16" s="6"/>
+      <c r="BD16" s="7"/>
+      <c r="BE16" s="6"/>
+      <c r="BF16" s="7"/>
+      <c r="BG16" s="6"/>
       <c r="BH16" s="3"/>
     </row>
     <row r="17" spans="7:60" ht="32.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1196,13 +1113,13 @@
       <c r="AI17" s="45"/>
       <c r="AJ17" s="61"/>
       <c r="BA17" s="1"/>
-      <c r="BB17" s="2"/>
-      <c r="BC17" s="1"/>
-      <c r="BD17" s="2"/>
-      <c r="BE17" s="1"/>
-      <c r="BF17" s="2"/>
-      <c r="BG17" s="1"/>
-      <c r="BH17" s="2"/>
+      <c r="BB17" s="4"/>
+      <c r="BC17" s="64"/>
+      <c r="BD17" s="65"/>
+      <c r="BE17" s="66"/>
+      <c r="BF17" s="65"/>
+      <c r="BG17" s="67"/>
+      <c r="BH17" s="62"/>
     </row>
     <row r="18" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G18" s="2"/>
@@ -1234,13 +1151,13 @@
       <c r="AI18" s="53"/>
       <c r="AJ18" s="48"/>
       <c r="BA18" s="2"/>
-      <c r="BB18" s="3"/>
-      <c r="BC18" s="2"/>
+      <c r="BB18" s="5"/>
+      <c r="BC18" s="68"/>
       <c r="BD18" s="3"/>
       <c r="BE18" s="2"/>
       <c r="BF18" s="3"/>
-      <c r="BG18" s="2"/>
-      <c r="BH18" s="3"/>
+      <c r="BG18" s="69"/>
+      <c r="BH18" s="63"/>
     </row>
     <row r="19" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G19" s="1"/>
@@ -1272,13 +1189,13 @@
       <c r="AI19" s="48"/>
       <c r="AJ19" s="61"/>
       <c r="BA19" s="1"/>
-      <c r="BB19" s="2"/>
-      <c r="BC19" s="1"/>
+      <c r="BB19" s="4"/>
+      <c r="BC19" s="70"/>
       <c r="BD19" s="2"/>
       <c r="BE19" s="1"/>
       <c r="BF19" s="2"/>
-      <c r="BG19" s="1"/>
-      <c r="BH19" s="2"/>
+      <c r="BG19" s="71"/>
+      <c r="BH19" s="62"/>
     </row>
     <row r="20" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G20" s="2"/>
@@ -1310,15 +1227,15 @@
       <c r="AI20" s="53"/>
       <c r="AJ20" s="48"/>
       <c r="BA20" s="2"/>
-      <c r="BB20" s="3"/>
-      <c r="BC20" s="2"/>
+      <c r="BB20" s="5"/>
+      <c r="BC20" s="68"/>
       <c r="BD20" s="3"/>
       <c r="BE20" s="2"/>
       <c r="BF20" s="3"/>
-      <c r="BG20" s="2"/>
-      <c r="BH20" s="3"/>
-    </row>
-    <row r="21" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG20" s="69"/>
+      <c r="BH20" s="63"/>
+    </row>
+    <row r="21" spans="7:60" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>
@@ -1348,13 +1265,13 @@
       <c r="AI21" s="48"/>
       <c r="AJ21" s="61"/>
       <c r="BA21" s="1"/>
-      <c r="BB21" s="2"/>
-      <c r="BC21" s="1"/>
-      <c r="BD21" s="2"/>
-      <c r="BE21" s="1"/>
-      <c r="BF21" s="2"/>
-      <c r="BG21" s="1"/>
-      <c r="BH21" s="2"/>
+      <c r="BB21" s="4"/>
+      <c r="BC21" s="72"/>
+      <c r="BD21" s="73"/>
+      <c r="BE21" s="74"/>
+      <c r="BF21" s="73"/>
+      <c r="BG21" s="75"/>
+      <c r="BH21" s="62"/>
     </row>
     <row r="22" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G22" s="2"/>
@@ -1387,11 +1304,11 @@
       <c r="AJ22" s="48"/>
       <c r="BA22" s="2"/>
       <c r="BB22" s="3"/>
-      <c r="BC22" s="2"/>
-      <c r="BD22" s="3"/>
-      <c r="BE22" s="2"/>
-      <c r="BF22" s="3"/>
-      <c r="BG22" s="2"/>
+      <c r="BC22" s="8"/>
+      <c r="BD22" s="9"/>
+      <c r="BE22" s="8"/>
+      <c r="BF22" s="9"/>
+      <c r="BG22" s="8"/>
       <c r="BH22" s="3"/>
     </row>
     <row r="23" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1651,6 +1568,5 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the video of demosaicking_1 is OK
</commit_message>
<xml_diff>
--- a/Demosaic/sketchMap.xlsx
+++ b/Demosaic/sketchMap.xlsx
@@ -14,13 +14,118 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>G1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -560,6 +665,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -842,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:BH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="BD17" sqref="BD17"/>
+    <sheetView tabSelected="1" topLeftCell="AS23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="BG26" sqref="BG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1349,7 +1484,7 @@
       <c r="BG23" s="1"/>
       <c r="BH23" s="2"/>
     </row>
-    <row r="24" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:60" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G24" s="2"/>
       <c r="H24" s="3"/>
       <c r="I24" s="2"/>
@@ -1408,6 +1543,21 @@
       <c r="AH25" s="37"/>
       <c r="AI25" s="52"/>
       <c r="AJ25" s="61"/>
+      <c r="BA25" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB25" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC25" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD25" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="BE25" s="78" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="7:60" ht="32.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="P26" s="3"/>
@@ -1430,8 +1580,39 @@
       <c r="AH26" s="51"/>
       <c r="AI26" s="51"/>
       <c r="AJ26" s="60"/>
-    </row>
-    <row r="27" spans="7:60" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+      <c r="BA26" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB26" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="BC26" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="BD26" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="BE26" s="82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="7:60" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BA27" s="79" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB27" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC27" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="BD27" s="81" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE27" s="82" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="28" spans="7:60" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AA28" s="42"/>
       <c r="AB28" s="28"/>
@@ -1443,8 +1624,23 @@
       <c r="AH28" s="28"/>
       <c r="AI28" s="55"/>
       <c r="AJ28" s="30"/>
-    </row>
-    <row r="29" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BA28" s="79" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB28" s="81" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC28" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="BD28" s="81" t="s">
+        <v>18</v>
+      </c>
+      <c r="BE28" s="82" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="7:60" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AA29" s="31"/>
       <c r="AB29" s="27"/>
       <c r="AC29" s="28"/>
@@ -1455,6 +1651,21 @@
       <c r="AH29" s="29"/>
       <c r="AI29" s="30"/>
       <c r="AJ29" s="61"/>
+      <c r="BA29" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB29" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="BC29" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="BD29" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="BE29" s="85" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" spans="7:60" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA30" s="57"/>

</xml_diff>

<commit_message>
train model for DJDD
</commit_message>
<xml_diff>
--- a/Demosaic/sketchMap.xlsx
+++ b/Demosaic/sketchMap.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISP\PersonalProjects\ISPAlgorithmStudy\Demosaic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fred\ISP\ISPAlgorithmStudy\Demosaic\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EFF9A0-D8FE-4CBA-8F0D-E1416E52308D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1006,11 +1007,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G2:BH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS29" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AY30" sqref="AY30"/>
+    <sheetView tabSelected="1" topLeftCell="AS14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="BK16" sqref="BK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
the note of demosaicking is OK
</commit_message>
<xml_diff>
--- a/Demosaic/sketchMap.xlsx
+++ b/Demosaic/sketchMap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Fred\ISP\ISPAlgorithmStudy\Demosaic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EFF9A0-D8FE-4CBA-8F0D-E1416E52308D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC36173-7ADF-4919-BCC7-1892E536B8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -686,36 +686,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -726,6 +696,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1010,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G2:BH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="BK16" sqref="BK16"/>
+    <sheetView tabSelected="1" topLeftCell="AS23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AY26" sqref="AY26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1576,19 +1585,19 @@
       <c r="AH25" s="37"/>
       <c r="AI25" s="52"/>
       <c r="AJ25" s="61"/>
-      <c r="BA25" s="76" t="s">
+      <c r="BA25" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="BB25" s="77" t="s">
+      <c r="BB25" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="BC25" s="77" t="s">
+      <c r="BC25" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="BD25" s="77" t="s">
+      <c r="BD25" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="BE25" s="78" t="s">
+      <c r="BE25" s="82" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1613,36 +1622,36 @@
       <c r="AH26" s="51"/>
       <c r="AI26" s="51"/>
       <c r="AJ26" s="60"/>
-      <c r="BA26" s="79" t="s">
+      <c r="BA26" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="BB26" s="80" t="s">
+      <c r="BB26" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="BC26" s="80" t="s">
+      <c r="BC26" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="BD26" s="81" t="s">
+      <c r="BD26" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="BE26" s="82" t="s">
+      <c r="BE26" s="92" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="7:60" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="BA27" s="79" t="s">
+      <c r="BA27" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="BB27" s="80" t="s">
+      <c r="BB27" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="BC27" s="80" t="s">
+      <c r="BC27" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="BD27" s="81" t="s">
+      <c r="BD27" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="BE27" s="82" t="s">
+      <c r="BE27" s="84" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1657,19 +1666,19 @@
       <c r="AH28" s="28"/>
       <c r="AI28" s="55"/>
       <c r="AJ28" s="30"/>
-      <c r="BA28" s="79" t="s">
+      <c r="BA28" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="BB28" s="81" t="s">
+      <c r="BB28" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="BC28" s="81" t="s">
+      <c r="BC28" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="BD28" s="81" t="s">
+      <c r="BD28" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="BE28" s="82" t="s">
+      <c r="BE28" s="92" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1684,19 +1693,19 @@
       <c r="AH29" s="29"/>
       <c r="AI29" s="30"/>
       <c r="AJ29" s="61"/>
-      <c r="BA29" s="83" t="s">
+      <c r="BA29" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="BB29" s="84" t="s">
+      <c r="BB29" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="BC29" s="84" t="s">
+      <c r="BC29" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="BD29" s="84" t="s">
+      <c r="BD29" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="BE29" s="85" t="s">
+      <c r="BE29" s="87" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1757,19 +1766,19 @@
       <c r="AH33" s="26"/>
       <c r="AI33" s="34"/>
       <c r="AJ33" s="61"/>
-      <c r="BA33" s="86" t="s">
+      <c r="BA33" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="BB33" s="87" t="s">
+      <c r="BB33" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="BC33" s="88" t="s">
+      <c r="BC33" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="BD33" s="87" t="s">
+      <c r="BD33" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="BE33" s="89" t="s">
+      <c r="BE33" s="79" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>